<commit_message>
working with text valitation
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\OneDrive - UNIVERSIDAD NACIONAL DE INGENIERIA\Venado\Cris\SapHunter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\RobotDaniel\VENADO\SapHunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D4D520-5A73-487F-936E-0BA9E99DBB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91EB278-5646-432A-8067-B9B70D65792B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bancos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">cuentas!$A$1:$K$37</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,12 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="113">
   <si>
     <t>BCP</t>
   </si>
@@ -373,7 +370,13 @@
     <t>A2</t>
   </si>
   <si>
-    <t>D:\Program Files (x86)\ERPSAP\SAPgui\saplogon.exe</t>
+    <t>ModoValidacion</t>
+  </si>
+  <si>
+    <t>Doble</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\SAP\FrontEnd\SAPgui\saplogon.exe</t>
   </si>
 </sst>
 </file>
@@ -775,19 +778,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" customWidth="1"/>
+    <col min="13" max="13" width="24.6640625" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="10" t="s">
         <v>22</v>
       </c>
@@ -834,7 +837,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>51</v>
       </c>
@@ -884,7 +887,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
@@ -934,7 +937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>58</v>
       </c>
@@ -984,7 +987,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>83</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>88</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>65</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>109</v>
       </c>
@@ -1174,18 +1177,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36875E07-AEFE-4371-8D99-4CC952440A1F}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>102</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>96</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>97</v>
       </c>
@@ -1209,7 +1212,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -1217,12 +1220,20 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
       <c r="B5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>110</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1239,12 +1250,12 @@
       <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>95</v>
       </c>
@@ -1279,7 +1290,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1312,7 +1323,7 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1345,7 +1356,7 @@
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1378,7 +1389,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1411,7 +1422,7 @@
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1444,7 +1455,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
@@ -1477,7 +1488,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1510,7 +1521,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1543,7 +1554,7 @@
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1576,7 +1587,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>10</v>
       </c>
@@ -1609,7 +1620,7 @@
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1642,7 +1653,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
@@ -1675,7 +1686,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1708,7 +1719,7 @@
       </c>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1741,7 +1752,7 @@
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -1774,7 +1785,7 @@
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <v>16</v>
       </c>
@@ -1807,7 +1818,7 @@
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1840,7 +1851,7 @@
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1873,7 +1884,7 @@
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -1906,7 +1917,7 @@
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>20</v>
       </c>
@@ -1939,7 +1950,7 @@
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -1972,7 +1983,7 @@
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2005,7 +2016,7 @@
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2038,7 +2049,7 @@
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -2071,7 +2082,7 @@
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2104,7 +2115,7 @@
       </c>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
         <v>26</v>
       </c>
@@ -2137,7 +2148,7 @@
       </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2170,7 +2181,7 @@
       </c>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
         <v>28</v>
       </c>
@@ -2203,7 +2214,7 @@
       </c>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2236,7 +2247,7 @@
       </c>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>30</v>
       </c>
@@ -2269,7 +2280,7 @@
       </c>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2302,7 +2313,7 @@
       </c>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2335,7 +2346,7 @@
       </c>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
         <v>33</v>
       </c>
@@ -2368,7 +2379,7 @@
       </c>
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
         <v>34</v>
       </c>
@@ -2401,7 +2412,7 @@
       </c>
       <c r="K35" s="6"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
         <v>35</v>
       </c>
@@ -2434,7 +2445,7 @@
       </c>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
ready to monday production
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\Bot1\SapHunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39E6131-6B5B-40AD-8F22-F5441CD87C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC1F1BD-3E4B-4540-8552-A606B18342C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bancos" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>banco bisa.xlsx</t>
   </si>
   <si>
-    <t>A6</t>
-  </si>
-  <si>
     <t>10000020161539</t>
   </si>
   <si>
@@ -401,6 +398,9 @@
   </si>
   <si>
     <t>PRD SAP HANA</t>
+  </si>
+  <si>
+    <t>B17</t>
   </si>
 </sst>
 </file>
@@ -811,78 +811,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="18.42578125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="20.7109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" customWidth="1"/>
     <col min="16" max="16" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O1" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P1" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -891,16 +891,16 @@
         <v>3</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
@@ -912,13 +912,13 @@
         <v>2</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
         <v>35</v>
       </c>
       <c r="P2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -926,7 +926,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -962,10 +962,10 @@
         <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P3" t="s">
         <v>0</v>
@@ -973,10 +973,10 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1006,24 +1006,24 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M4" t="s">
-        <v>105</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="O4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1056,24 +1056,24 @@
         <v>3</v>
       </c>
       <c r="L5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="O5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1106,27 +1106,27 @@
         <v>3</v>
       </c>
       <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" t="s">
         <v>38</v>
       </c>
-      <c r="M6" t="s">
-        <v>39</v>
-      </c>
       <c r="N6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1162,18 +1162,18 @@
         <v>1</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1245,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36875E07-AEFE-4371-8D99-4CC952440A1F}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,82 +1258,82 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>100</v>
-      </c>
       <c r="D1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B7" s="13"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
         <v>113</v>
-      </c>
-      <c r="B8" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,37 +1369,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1407,31 +1407,31 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D2" s="7">
         <v>120161539</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="G2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="6"/>
     </row>
@@ -1440,7 +1440,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>0</v>
@@ -1449,22 +1449,22 @@
         <v>2015026265385</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J3" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -1473,31 +1473,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" s="7">
         <v>4010501329</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J4" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -1506,31 +1506,31 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D5" s="7">
         <v>4010066211</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J5" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -1539,31 +1539,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="7">
         <v>4010599686</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J6" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -1572,31 +1572,31 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="7">
         <v>4010374232</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1605,31 +1605,31 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="7">
         <v>4010395865</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="H8" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K8" s="6"/>
     </row>
@@ -1638,31 +1638,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="7">
         <v>100070014</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J9" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K9" s="6"/>
     </row>
@@ -1671,7 +1671,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>0</v>
@@ -1680,22 +1680,22 @@
         <v>7015089120389</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="J10" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K10" s="6"/>
     </row>
@@ -1704,31 +1704,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7">
         <v>100072017</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F11" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="J11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K11" s="6"/>
     </row>
@@ -1737,31 +1737,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="7">
         <v>100070022</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K12" s="6"/>
     </row>
@@ -1770,31 +1770,31 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="7">
         <v>100070031</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1803,31 +1803,31 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="7">
         <v>100070049</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K14" s="6"/>
     </row>
@@ -1836,31 +1836,31 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="7">
         <v>100070057</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K15" s="6"/>
     </row>
@@ -1869,31 +1869,31 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D16" s="7">
         <v>100070065</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K16" s="6"/>
     </row>
@@ -1902,31 +1902,31 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D17" s="7">
         <v>100070073</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1935,31 +1935,31 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="7">
         <v>100070081</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K18" s="6"/>
     </row>
@@ -1968,31 +1968,31 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D19" s="7">
         <v>100070090</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K19" s="6"/>
     </row>
@@ -2001,31 +2001,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D20" s="7">
         <v>100070103</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K20" s="6"/>
     </row>
@@ -2034,31 +2034,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D21" s="7">
         <v>100070111</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -2067,31 +2067,31 @@
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="8">
         <v>100070049</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -2100,31 +2100,31 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" s="7">
         <v>100070065</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K23" s="6"/>
     </row>
@@ -2133,31 +2133,31 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24" s="7">
         <v>100070090</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K24" s="6"/>
     </row>
@@ -2166,31 +2166,31 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D25" s="7">
         <v>100070103</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K25" s="6"/>
     </row>
@@ -2199,31 +2199,31 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="7">
         <v>100070111</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K26" s="6"/>
     </row>
@@ -2232,31 +2232,31 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="D27" s="7">
         <v>2120271437</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I27" s="6" t="s">
-        <v>82</v>
-      </c>
       <c r="J27" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K27" s="6"/>
     </row>
@@ -2265,31 +2265,31 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28" s="7">
         <v>620210</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K28" s="6"/>
     </row>
@@ -2298,31 +2298,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D29" s="7">
         <v>61121267099</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K29" s="6"/>
     </row>
@@ -2331,7 +2331,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>0</v>
@@ -2340,22 +2340,22 @@
         <v>7015054675359</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K30" s="6"/>
     </row>
@@ -2364,31 +2364,31 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" s="7">
         <v>2041320635</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K31" s="6"/>
     </row>
@@ -2397,31 +2397,31 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="7">
         <v>4010132476</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K32" s="6"/>
     </row>
@@ -2430,31 +2430,31 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D33" s="7">
         <v>4010542984</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K33" s="6"/>
     </row>
@@ -2463,31 +2463,31 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="7">
         <v>4010678183</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K34" s="6"/>
     </row>
@@ -2496,31 +2496,31 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D35" s="7">
         <v>4010640108</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K35" s="6"/>
     </row>
@@ -2529,31 +2529,31 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D36" s="7">
         <v>7934540012</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K36" s="6"/>
     </row>
@@ -2562,32 +2562,32 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D37" s="7">
         <v>7934542015</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ready to 2 day prd
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://industriasvenado-my.sharepoint.com/personal/felipevillarroel_grupovenado_com/Documents/Proyecto Automatización Procesos Contables y Tesoreria/Bot1/SapHunter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DanielBots\Bot1\SapHunter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{78AD2E3F-83EB-4AFD-89CF-3B639CED8CED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D4B640E-BB39-4E3E-ABAC-587AA998AAF2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8662B7-E1AF-4762-8F68-B22EDC6FF81C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="12240" windowHeight="8640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bancos" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="109">
   <si>
     <t>CeldaPeriodo</t>
   </si>
@@ -76,9 +76,6 @@
     <t xml:space="preserve"> Info. Complementaria</t>
   </si>
   <si>
-    <t>NombreHoja</t>
-  </si>
-  <si>
     <t>CuentaCol</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>UNION</t>
-  </si>
-  <si>
     <t>10000020161539</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>A13</t>
   </si>
   <si>
-    <t>MERCANTIL</t>
-  </si>
-  <si>
     <t>4010066211</t>
   </si>
   <si>
@@ -136,9 +127,6 @@
     <t>B20</t>
   </si>
   <si>
-    <t>Sheet</t>
-  </si>
-  <si>
     <t>620210</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
     <t>A18</t>
   </si>
   <si>
-    <t>Extracto</t>
-  </si>
-  <si>
     <t>2041320635</t>
   </si>
   <si>
@@ -160,9 +145,6 @@
     <t>A2</t>
   </si>
   <si>
-    <t>BISA</t>
-  </si>
-  <si>
     <t>0100070014</t>
   </si>
   <si>
@@ -383,13 +365,16 @@
   </si>
   <si>
     <t>AUN NO HABILITADA EN SISTEMA</t>
+  </si>
+  <si>
+    <t>CAMPO ITF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -793,19 +778,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="24.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" customWidth="1"/>
     <col min="15" max="15" width="20.7109375" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
@@ -840,24 +825,24 @@
         <v>10</v>
       </c>
       <c r="M1" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="10" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="11" t="s">
+      <c r="B2" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
       </c>
       <c r="C2">
         <v>7</v>
@@ -866,10 +851,10 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -878,36 +863,36 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2">
         <v>3</v>
       </c>
       <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2">
+        <v>3</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="B3" t="s">
         <v>20</v>
-      </c>
-      <c r="P2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -916,10 +901,10 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3">
         <v>20</v>
@@ -928,36 +913,36 @@
         <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3">
         <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O3" t="s">
+      <c r="B4" t="s">
         <v>24</v>
-      </c>
-      <c r="P3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -972,7 +957,7 @@
         <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4">
         <v>21</v>
@@ -987,27 +972,27 @@
         <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>30</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1022,42 +1007,42 @@
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5">
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5">
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <v>6</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="11" t="s">
-        <v>33</v>
-      </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1066,10 +1051,10 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6">
         <v>12</v>
@@ -1078,36 +1063,36 @@
         <v>13</v>
       </c>
       <c r="I6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J6">
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
       </c>
       <c r="C7">
         <v>3</v>
@@ -1116,10 +1101,10 @@
         <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -1128,33 +1113,33 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7">
         <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7">
         <v>7</v>
       </c>
-      <c r="M7" t="s">
-        <v>39</v>
+      <c r="M7">
+        <v>4</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" hidden="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1163,10 +1148,10 @@
         <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -1175,18 +1160,18 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J8">
         <v>4</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" hidden="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -1195,10 +1180,10 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9">
         <v>6</v>
@@ -1207,13 +1192,13 @@
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J9">
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1226,99 +1211,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36875E07-AEFE-4371-8D99-4CC952440A1F}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="F2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="12" t="s">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="B3" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>47</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>50</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="12" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="13"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>60</v>
-      </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{694602D6-F8AF-4958-A87C-CDA5EC5C67E2}">
       <formula1>$F$2:$F$4</formula1>
     </dataValidation>
@@ -1337,1242 +1322,1249 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45A073E-2743-4135-ADF5-D2E575AFBED5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="7">
         <v>120161539</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="8">
         <v>2015026265385</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7">
         <v>4010501329</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="7">
         <v>4010066211</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K5" s="6"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="7">
         <v>4010599686</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="7">
         <v>4010374232</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="7">
         <v>4010395865</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7">
         <v>100070014</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K9" s="6"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="7">
         <v>7015089120389</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11" s="7">
         <v>100072017</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>91</v>
-      </c>
       <c r="J11" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K11" s="6"/>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D12" s="7">
         <v>100070022</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" s="7">
         <v>100070031</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D14" s="7">
         <v>100070049</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K14" s="6"/>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D15" s="7">
         <v>100070057</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K15" s="6"/>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D16" s="7">
         <v>100070065</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D17" s="7">
         <v>100070073</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D18" s="7">
         <v>100070081</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D19" s="7">
         <v>100070090</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D20" s="7">
         <v>100070103</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D21" s="7">
         <v>100070111</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>21</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D22" s="8">
         <v>100070049</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D23" s="7">
         <v>100070065</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D24" s="7">
         <v>100070090</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D25" s="7">
         <v>100070103</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D26" s="7">
         <v>100070111</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="7">
         <v>2120271437</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D28" s="7">
         <v>620210</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D29" s="7">
         <v>61121267099</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D30" s="7">
         <v>7015054675359</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D31" s="7">
         <v>2041320635</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D32" s="7">
         <v>4010132476</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K32" s="6"/>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D33" s="7">
         <v>4010542984</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K33" s="6"/>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D34" s="7">
         <v>4010678183</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K34" s="6"/>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D35" s="7">
         <v>4010640108</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K35" s="6"/>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D36" s="7">
         <v>7934540012</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K36" s="6"/>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D37" s="7">
         <v>7934542015</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F37" s="6"/>
       <c r="G37" s="6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K37" xr:uid="{E45A073E-2743-4135-ADF5-D2E575AFBED5}"/>
+  <autoFilter ref="A1:K37" xr:uid="{E45A073E-2743-4135-ADF5-D2E575AFBED5}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Fassil"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Haz clic e introduce un valor de intervalo 'Hoja 1'!Q1:Q15" sqref="C2:C37" xr:uid="{70345916-44DB-4C25-A750-ECDBBC8F479B}">
       <formula1>$V$1:$V$13</formula1>

</xml_diff>